<commit_message>
New and updated specs.
</commit_message>
<xml_diff>
--- a/spec/ConvSpec-3XX-v2.4.xlsx
+++ b/spec/ConvSpec-3XX-v2.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevinford\work\marc2bibframe2\spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E503171D-720C-468E-B493-F42828674166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6322C9EB-1981-4DAF-911A-AFF11EF9B5F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2010,7 +2010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D610"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D558" sqref="D558"/>
     </sheetView>
   </sheetViews>

</xml_diff>